<commit_message>
writeup updated; more results
</commit_message>
<xml_diff>
--- a/finalproject/write-up/score data.xlsx
+++ b/finalproject/write-up/score data.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="41">
   <si>
     <t>Algorithm</t>
   </si>
@@ -156,6 +156,27 @@
   </si>
   <si>
     <t>CapThres=-100, buf=10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline </t>
+  </si>
+  <si>
+    <t>200 moves</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>Thres=-100, scaredTime=10</t>
+  </si>
+  <si>
+    <t>Thres=-125, time=10</t>
+  </si>
+  <si>
+    <t>50 moves</t>
+  </si>
+  <si>
+    <t>Thres=-150, time=10</t>
   </si>
 </sst>
 </file>
@@ -217,8 +238,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -261,7 +288,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -280,6 +307,9 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -298,6 +328,9 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1047,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AF41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1064,6 +1097,9 @@
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D1" t="s">
         <v>24</v>
       </c>
@@ -1920,6 +1956,348 @@
       <c r="AF14" s="2">
         <f>AVERAGE(AF3:AF12)</f>
         <v>498.90772301515</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1264.13553112</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1264.13553112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1092.4423876599999</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1092.4423876599999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2">
+        <v>648.60251877799999</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>648.60251877799999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2">
+        <v>255.41149254199999</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2">
+        <v>255.41149254199999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1">
+        <v>5</v>
+      </c>
+      <c r="B24" s="2">
+        <v>30.087156974500001</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>579.61181571700001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2">
+        <v>999.81892902100003</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2">
+        <v>999.81892902100003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2">
+        <v>862.66004696499999</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26" s="2">
+        <v>562.50617603499995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1">
+        <v>8</v>
+      </c>
+      <c r="B27" s="2">
+        <v>600.16129394200004</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2">
+        <v>600.16129394200004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1">
+        <v>9</v>
+      </c>
+      <c r="B28" s="2">
+        <v>901.04026481000005</v>
+      </c>
+      <c r="D28">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2">
+        <v>901.04026481000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1">
+        <v>10</v>
+      </c>
+      <c r="B29" s="2">
+        <v>467.28570589899999</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
+        <v>818.49615234400005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1">
+        <v>11</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1090.1498091399999</v>
+      </c>
+      <c r="D30">
+        <v>11</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1086.03281528</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1">
+        <v>12</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1115.01770145</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31" s="2">
+        <v>839.06133802199997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1">
+        <v>13</v>
+      </c>
+      <c r="B32" s="2">
+        <v>814.80119441399995</v>
+      </c>
+      <c r="D32">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2">
+        <v>736.97497188399996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1">
+        <v>14</v>
+      </c>
+      <c r="B33" s="2">
+        <v>909.62100499500002</v>
+      </c>
+      <c r="D33">
+        <v>14</v>
+      </c>
+      <c r="E33" s="2">
+        <v>909.62100499500002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1">
+        <v>15</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2049.4600154</v>
+      </c>
+      <c r="D34">
+        <v>15</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2049.4600154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1">
+        <v>16</v>
+      </c>
+      <c r="B35" s="2">
+        <v>942.70378424900002</v>
+      </c>
+      <c r="D35">
+        <v>16</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1084.4743467799999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1">
+        <v>17</v>
+      </c>
+      <c r="B36" s="2">
+        <v>531.50877935200003</v>
+      </c>
+      <c r="D36">
+        <v>17</v>
+      </c>
+      <c r="E36" s="2">
+        <v>845.61834408200002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1">
+        <v>18</v>
+      </c>
+      <c r="B37" s="2">
+        <v>313.75163984</v>
+      </c>
+      <c r="D37">
+        <v>18</v>
+      </c>
+      <c r="E37" s="2">
+        <v>313.75163984</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1">
+        <v>19</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1639.8191200199999</v>
+      </c>
+      <c r="D38">
+        <v>19</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1639.8191200199999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1">
+        <v>20</v>
+      </c>
+      <c r="B39" s="2">
+        <v>573.486980432</v>
+      </c>
+      <c r="D39">
+        <v>20</v>
+      </c>
+      <c r="E39" s="2">
+        <v>407.148412742</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2">
+        <f>AVERAGE(B20:B39)</f>
+        <v>855.09826785017526</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="2">
+        <f>AVERAGE(E20:E39)</f>
+        <v>881.70942855070007</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H41" s="2" t="e">
+        <f>AVERAGE(H20:H39)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final project code done
</commit_message>
<xml_diff>
--- a/finalproject/write-up/score data.xlsx
+++ b/finalproject/write-up/score data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="0" windowWidth="23660" windowHeight="14540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="860" yWindow="0" windowWidth="24740" windowHeight="14580" tabRatio="460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Single runs" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,9 @@
     <sheet name="Rollup" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="scores" localSheetId="3">Sheet2!$A$4:$AY$23</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -55,8 +58,72 @@
 </comments>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="scores.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:wihl:Projects:Courses:Harvard CS181 Spring 2014:finalproject:final_project_code_mac:scores.txt" space="1" comma="1" consecutive="1">
+      <textFields count="53">
+        <textField type="skip"/>
+        <textField/>
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="59">
   <si>
     <t>Algorithm</t>
   </si>
@@ -233,9 +300,6 @@
   </si>
   <si>
     <t>Seed vs Score</t>
-  </si>
-  <si>
-    <t>Scores</t>
   </si>
 </sst>
 </file>
@@ -1340,6 +1404,393 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Cambria Math"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Cambria Math"/>
+              </a:rPr>
+              <a:t>Scores</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Cambria Math"/>
+              </a:rPr>
+              <a:t> vs Seed (50 games,  200 moves)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Cambria Math"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$AZ$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$AZ$4:$AZ$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1221.495886364072</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>804.32283700986</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>780.07274559926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>586.2960089943399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>476.5668460347221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>835.3629512892761</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>902.06746599216</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1235.045439546108</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>885.672847247098</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>477.118445305508</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1702.242636050979</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>712.941859378744</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>975.140420474018</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>931.5983324125242</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1450.00965090558</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>655.4359881080978</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>938.5178521367327</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>562.278350617004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>913.7319797826603</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>967.81339172117</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$BA$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$BA$4:$BA$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>-6731.5967488</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4114.53113566</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4396.83610056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1738.99796766</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5397.80046983</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2653.62732383</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3207.18268061</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2540.22562643</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5240.2722558</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6063.46697992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2402.29151027</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-6963.83323014</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2280.2401987</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2497.27882063</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-6182.60285995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4584.73722151</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2785.29421232</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-6803.39602197</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-6781.15585602</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-5439.94967932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$BB$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$BB$4:$BB$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5141.20009898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4186.33245004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3996.79701716</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5325.38718527</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3966.33229926</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5130.44759424</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3895.16456433</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4700.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4062.92707975</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3751.5658674</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7438.06575536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6180.86896378</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4520.54831675</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4385.4647865</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6067.92393353</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3316.62240907</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4552.27811332</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3027.83792801</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6819.14577542</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4677.12333693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2088144488"/>
+        <c:axId val="-2088162168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2088144488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2088162168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2088162168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2088144488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1403,6 +1854,45 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scores" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4891,129 +5381,3384 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane xSplit="13920" topLeftCell="AY1" activePane="topRight"/>
+      <selection activeCell="AR1" sqref="AR1"/>
+      <selection pane="topRight" activeCell="AZ3" sqref="AZ3:BB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="52" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:54">
       <c r="A1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:54">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="AZ3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54">
       <c r="A4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4">
+        <v>-751.14046163700004</v>
+      </c>
+      <c r="C4">
+        <v>1944.52507687</v>
+      </c>
+      <c r="D4">
+        <v>4449.7399132700002</v>
+      </c>
+      <c r="E4">
+        <v>2508.3813727800002</v>
+      </c>
+      <c r="F4">
+        <v>712.10372485899995</v>
+      </c>
+      <c r="G4">
+        <v>2676.7608503800002</v>
+      </c>
+      <c r="H4">
+        <v>1568.6078989299999</v>
+      </c>
+      <c r="I4">
+        <v>3465.87344089</v>
+      </c>
+      <c r="J4">
+        <v>-671.03177937299995</v>
+      </c>
+      <c r="K4">
+        <v>2250.66292363</v>
+      </c>
+      <c r="L4">
+        <v>2074.6649830000001</v>
+      </c>
+      <c r="M4">
+        <v>3239.9188622500001</v>
+      </c>
+      <c r="N4">
+        <v>4488.6846156299998</v>
+      </c>
+      <c r="O4">
+        <v>-939.41682067800002</v>
+      </c>
+      <c r="P4">
+        <v>2486.4477286000001</v>
+      </c>
+      <c r="Q4">
+        <v>-1529.3742503399999</v>
+      </c>
+      <c r="R4">
+        <v>-2708.8951895800001</v>
+      </c>
+      <c r="S4">
+        <v>1448.7449414600001</v>
+      </c>
+      <c r="T4">
+        <v>2718.5552471400001</v>
+      </c>
+      <c r="U4">
+        <v>1310.6812647500001</v>
+      </c>
+      <c r="V4">
+        <v>2158.3289642499999</v>
+      </c>
+      <c r="W4">
+        <v>1764.13028614</v>
+      </c>
+      <c r="X4">
+        <v>1637.3483387799999</v>
+      </c>
+      <c r="Y4">
+        <v>2236.83388754</v>
+      </c>
+      <c r="Z4">
+        <v>242.718583306</v>
+      </c>
+      <c r="AA4">
+        <v>2046.7273806999999</v>
+      </c>
+      <c r="AB4">
+        <v>2838.09045771</v>
+      </c>
+      <c r="AC4">
+        <v>2329.7575277400001</v>
+      </c>
+      <c r="AD4">
+        <v>1926.1241009</v>
+      </c>
+      <c r="AE4">
+        <v>2183.3299570999998</v>
+      </c>
+      <c r="AF4">
+        <v>1873.1762349400001</v>
+      </c>
+      <c r="AG4">
+        <v>5141.2000989799999</v>
+      </c>
+      <c r="AH4">
+        <v>55.831344772599998</v>
+      </c>
+      <c r="AI4">
+        <v>1550.01854043</v>
+      </c>
+      <c r="AJ4">
+        <v>1100</v>
+      </c>
+      <c r="AK4">
+        <v>1169.27951282</v>
+      </c>
+      <c r="AL4">
+        <v>-4362.2144984300003</v>
+      </c>
+      <c r="AM4">
+        <v>1410.82927161</v>
+      </c>
+      <c r="AN4">
+        <v>522.008598624</v>
+      </c>
+      <c r="AO4">
+        <v>-2402.9150268399999</v>
+      </c>
+      <c r="AP4">
+        <v>1635.5135903</v>
+      </c>
+      <c r="AQ4">
+        <v>3622.65084798</v>
+      </c>
+      <c r="AR4">
+        <v>-6731.5967487999997</v>
+      </c>
+      <c r="AS4">
+        <v>-1094.3821736699999</v>
+      </c>
+      <c r="AT4">
+        <v>1673.3867490600001</v>
+      </c>
+      <c r="AU4">
+        <v>816.427385383</v>
+      </c>
+      <c r="AV4">
+        <v>3667.4201798499998</v>
+      </c>
+      <c r="AW4">
+        <v>-495.17460519399998</v>
+      </c>
+      <c r="AX4">
+        <v>2424.91411036</v>
+      </c>
+      <c r="AY4">
+        <v>-609.46292096900004</v>
+      </c>
+      <c r="AZ4">
+        <f>AVERAGE(B4:AY4)</f>
+        <v>1221.4958863640722</v>
+      </c>
+      <c r="BA4">
+        <f>MIN(B4:AY4)</f>
+        <v>-6731.5967487999997</v>
+      </c>
+      <c r="BB4">
+        <f>MAX(B4:AY4)</f>
+        <v>5141.2000989799999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54">
       <c r="A5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="B5">
+        <v>1309.7279561800001</v>
+      </c>
+      <c r="C5">
+        <v>1814.4045563899999</v>
+      </c>
+      <c r="D5">
+        <v>915.25860838300002</v>
+      </c>
+      <c r="E5">
+        <v>311.81968291099997</v>
+      </c>
+      <c r="F5">
+        <v>2577.8736140199999</v>
+      </c>
+      <c r="G5">
+        <v>1404.1613567300001</v>
+      </c>
+      <c r="H5">
+        <v>2418.75817203</v>
+      </c>
+      <c r="I5">
+        <v>2269.9878776999999</v>
+      </c>
+      <c r="J5">
+        <v>1257.4708582999999</v>
+      </c>
+      <c r="K5">
+        <v>2632.6881112299998</v>
+      </c>
+      <c r="L5">
+        <v>1197.71142502</v>
+      </c>
+      <c r="M5">
+        <v>-1640.13889131</v>
+      </c>
+      <c r="N5">
+        <v>779.36327569499997</v>
+      </c>
+      <c r="O5">
+        <v>-3578.1180169899999</v>
+      </c>
+      <c r="P5">
+        <v>-236.46323970500001</v>
+      </c>
+      <c r="Q5">
+        <v>1015.96618495</v>
+      </c>
+      <c r="R5">
+        <v>679.11788008600001</v>
+      </c>
+      <c r="S5">
+        <v>1726.4152767999999</v>
+      </c>
+      <c r="T5">
+        <v>1548.3323451399999</v>
+      </c>
+      <c r="U5">
+        <v>2140.2381243200002</v>
+      </c>
+      <c r="V5">
+        <v>1050.88874035</v>
+      </c>
+      <c r="W5">
+        <v>1097.3493252000001</v>
+      </c>
+      <c r="X5">
+        <v>862.94159776900005</v>
+      </c>
+      <c r="Y5">
+        <v>410.21874407000001</v>
+      </c>
+      <c r="Z5">
+        <v>1498.7202379400001</v>
+      </c>
+      <c r="AA5">
+        <v>-3655.4963070700001</v>
+      </c>
+      <c r="AB5">
+        <v>-3503.5159701500002</v>
+      </c>
+      <c r="AC5">
+        <v>2320.1405190400001</v>
+      </c>
+      <c r="AD5">
+        <v>-910.82883184399998</v>
+      </c>
+      <c r="AE5">
+        <v>1684.11902237</v>
+      </c>
+      <c r="AF5">
+        <v>-1467.1782414700001</v>
+      </c>
+      <c r="AG5">
+        <v>3098.2991208399999</v>
+      </c>
+      <c r="AH5">
+        <v>307.52555036500002</v>
+      </c>
+      <c r="AI5">
+        <v>-2982.38911143</v>
+      </c>
+      <c r="AJ5">
+        <v>2373.87064091</v>
+      </c>
+      <c r="AK5">
+        <v>-4114.5311356599996</v>
+      </c>
+      <c r="AL5">
+        <v>1299.6838257100001</v>
+      </c>
+      <c r="AM5">
+        <v>2309.9056046199998</v>
+      </c>
+      <c r="AN5">
+        <v>809.25922485199999</v>
+      </c>
+      <c r="AO5">
+        <v>2185.9592094</v>
+      </c>
+      <c r="AP5">
+        <v>993.22287361600002</v>
+      </c>
+      <c r="AQ5">
+        <v>3027.90647885</v>
+      </c>
+      <c r="AR5">
+        <v>1031.3551632799999</v>
+      </c>
+      <c r="AS5">
+        <v>1098.96003277</v>
+      </c>
+      <c r="AT5">
+        <v>1422.0100623400001</v>
+      </c>
+      <c r="AU5">
+        <v>4186.3324500400004</v>
+      </c>
+      <c r="AV5">
+        <v>1616.4175655900001</v>
+      </c>
+      <c r="AW5">
+        <v>848.08100146300001</v>
+      </c>
+      <c r="AX5">
+        <v>-336.53960486800003</v>
+      </c>
+      <c r="AY5">
+        <v>1108.8789037199999</v>
+      </c>
+      <c r="AZ5">
+        <f t="shared" ref="AZ5:AZ23" si="0">AVERAGE(B5:AY5)</f>
+        <v>804.32283700986</v>
+      </c>
+      <c r="BA5">
+        <f t="shared" ref="BA5:BA23" si="1">MIN(B5:AY5)</f>
+        <v>-4114.5311356599996</v>
+      </c>
+      <c r="BB5">
+        <f t="shared" ref="BB5:BB23" si="2">MAX(B5:AY5)</f>
+        <v>4186.3324500400004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54">
       <c r="A6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6">
+        <v>1179.9158849999999</v>
+      </c>
+      <c r="C6">
+        <v>-788.61271220599997</v>
+      </c>
+      <c r="D6">
+        <v>-211.11189635900001</v>
+      </c>
+      <c r="E6">
+        <v>1926.8849455</v>
+      </c>
+      <c r="F6">
+        <v>1152.1700132399999</v>
+      </c>
+      <c r="G6">
+        <v>-1036.60814471</v>
+      </c>
+      <c r="H6">
+        <v>1022.43955204</v>
+      </c>
+      <c r="I6">
+        <v>3996.79701716</v>
+      </c>
+      <c r="J6">
+        <v>1595.1093597300001</v>
+      </c>
+      <c r="K6">
+        <v>-1110.9781778399999</v>
+      </c>
+      <c r="L6">
+        <v>-2078.7665774900001</v>
+      </c>
+      <c r="M6">
+        <v>1670.2202871300001</v>
+      </c>
+      <c r="N6">
+        <v>559.20412834700005</v>
+      </c>
+      <c r="O6">
+        <v>2016.7179387900001</v>
+      </c>
+      <c r="P6">
+        <v>1088.54912466</v>
+      </c>
+      <c r="Q6">
+        <v>94.946552346999994</v>
+      </c>
+      <c r="R6">
+        <v>1014.78767099</v>
+      </c>
+      <c r="S6">
+        <v>1833.3678827700001</v>
+      </c>
+      <c r="T6">
+        <v>1794.55191124</v>
+      </c>
+      <c r="U6">
+        <v>1300</v>
+      </c>
+      <c r="V6">
+        <v>540.61748992800005</v>
+      </c>
+      <c r="W6">
+        <v>772.51253695000003</v>
+      </c>
+      <c r="X6">
+        <v>1494.49924283</v>
+      </c>
+      <c r="Y6">
+        <v>1952.0677108699999</v>
+      </c>
+      <c r="Z6">
+        <v>-176.24564749999999</v>
+      </c>
+      <c r="AA6">
+        <v>26.889715413800001</v>
+      </c>
+      <c r="AB6">
+        <v>1346.0355811899999</v>
+      </c>
+      <c r="AC6">
+        <v>-1538.70027127</v>
+      </c>
+      <c r="AD6">
+        <v>137.76558122200001</v>
+      </c>
+      <c r="AE6">
+        <v>162.47961968300001</v>
+      </c>
+      <c r="AF6">
+        <v>2104.7174029900002</v>
+      </c>
+      <c r="AG6">
+        <v>1305.2370140999999</v>
+      </c>
+      <c r="AH6">
+        <v>224.03259078599999</v>
+      </c>
+      <c r="AI6">
+        <v>1615.2251328499999</v>
+      </c>
+      <c r="AJ6">
+        <v>2733.9818747499999</v>
+      </c>
+      <c r="AK6">
+        <v>2113.3910369499999</v>
+      </c>
+      <c r="AL6">
+        <v>-565.44855346999998</v>
+      </c>
+      <c r="AM6">
+        <v>-462.46089228900001</v>
+      </c>
+      <c r="AN6">
+        <v>3559.7710166299998</v>
+      </c>
+      <c r="AO6">
+        <v>2522.4697700299998</v>
+      </c>
+      <c r="AP6">
+        <v>1751.82897753</v>
+      </c>
+      <c r="AQ6">
+        <v>17.952708939200001</v>
+      </c>
+      <c r="AR6">
+        <v>-2530.7098664999999</v>
+      </c>
+      <c r="AS6">
+        <v>-4396.83610056</v>
+      </c>
+      <c r="AT6">
+        <v>950.98805147099995</v>
+      </c>
+      <c r="AU6">
+        <v>2794.5898945899999</v>
+      </c>
+      <c r="AV6">
+        <v>2007.5124635499999</v>
+      </c>
+      <c r="AW6">
+        <v>1060.8381842399999</v>
+      </c>
+      <c r="AX6">
+        <v>-1436.37944844</v>
+      </c>
+      <c r="AY6">
+        <v>1895.42970216</v>
+      </c>
+      <c r="AZ6">
+        <f t="shared" si="0"/>
+        <v>780.07274559925997</v>
+      </c>
+      <c r="BA6">
+        <f t="shared" si="1"/>
+        <v>-4396.83610056</v>
+      </c>
+      <c r="BB6">
+        <f t="shared" si="2"/>
+        <v>3996.79701716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54">
       <c r="A7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7">
+        <v>483.63932025000003</v>
+      </c>
+      <c r="C7">
+        <v>1028.9653825099999</v>
+      </c>
+      <c r="D7">
+        <v>502.62943247200002</v>
+      </c>
+      <c r="E7">
+        <v>1022.9155217799999</v>
+      </c>
+      <c r="F7">
+        <v>200.73328064399999</v>
+      </c>
+      <c r="G7">
+        <v>737.106520424</v>
+      </c>
+      <c r="H7">
+        <v>945.62976556900003</v>
+      </c>
+      <c r="I7">
+        <v>704.30571738000003</v>
+      </c>
+      <c r="J7">
+        <v>925.754053494</v>
+      </c>
+      <c r="K7">
+        <v>813.48279263300003</v>
+      </c>
+      <c r="L7">
+        <v>460.40002962599999</v>
+      </c>
+      <c r="M7">
+        <v>1282.6661251600001</v>
+      </c>
+      <c r="N7">
+        <v>-416.70418025200001</v>
+      </c>
+      <c r="O7">
+        <v>-1478.0480421</v>
+      </c>
+      <c r="P7">
+        <v>677.74219300499999</v>
+      </c>
+      <c r="Q7">
+        <v>152.370938666</v>
+      </c>
+      <c r="R7">
+        <v>507.41243458500003</v>
+      </c>
+      <c r="S7">
+        <v>988.93835048200003</v>
+      </c>
+      <c r="T7">
+        <v>2126.4685868699999</v>
+      </c>
+      <c r="U7">
+        <v>-1738.9979676600001</v>
+      </c>
+      <c r="V7">
+        <v>232.93696117900001</v>
+      </c>
+      <c r="W7">
+        <v>796.97214862400006</v>
+      </c>
+      <c r="X7">
+        <v>1406.06028846</v>
+      </c>
+      <c r="Y7">
+        <v>936.13905085199997</v>
+      </c>
+      <c r="Z7">
+        <v>-357.77240087799998</v>
+      </c>
+      <c r="AA7">
+        <v>1455.7763844999999</v>
+      </c>
+      <c r="AB7">
+        <v>198.65327444900001</v>
+      </c>
+      <c r="AC7">
+        <v>896.094205311</v>
+      </c>
+      <c r="AD7">
+        <v>1242.0543964399999</v>
+      </c>
+      <c r="AE7">
+        <v>1009.58531963</v>
+      </c>
+      <c r="AF7">
+        <v>715.59153026399997</v>
+      </c>
+      <c r="AG7">
+        <v>693.40027820700004</v>
+      </c>
+      <c r="AH7">
+        <v>-1624.18744064</v>
+      </c>
+      <c r="AI7">
+        <v>766.38977503499996</v>
+      </c>
+      <c r="AJ7">
+        <v>918.33668312400005</v>
+      </c>
+      <c r="AK7">
+        <v>1352.21474453</v>
+      </c>
+      <c r="AL7">
+        <v>854.10008518899997</v>
+      </c>
+      <c r="AM7">
+        <v>767.22284507200004</v>
+      </c>
+      <c r="AN7">
+        <v>-1093.69495351</v>
+      </c>
+      <c r="AO7">
+        <v>758.05492409299995</v>
+      </c>
+      <c r="AP7">
+        <v>-198.35803515699999</v>
+      </c>
+      <c r="AQ7">
+        <v>1100</v>
+      </c>
+      <c r="AR7">
+        <v>639.61901320699997</v>
+      </c>
+      <c r="AS7">
+        <v>341.95115643499997</v>
+      </c>
+      <c r="AT7">
+        <v>658.63817389099995</v>
+      </c>
+      <c r="AU7">
+        <v>391.443553296</v>
+      </c>
+      <c r="AV7">
+        <v>-1120.99812305</v>
+      </c>
+      <c r="AW7">
+        <v>-102.437062364</v>
+      </c>
+      <c r="AX7">
+        <v>428.21623271999999</v>
+      </c>
+      <c r="AY7">
+        <v>5325.3871852700004</v>
+      </c>
+      <c r="AZ7">
+        <f t="shared" si="0"/>
+        <v>586.2960089943399</v>
+      </c>
+      <c r="BA7">
+        <f t="shared" si="1"/>
+        <v>-1738.9979676600001</v>
+      </c>
+      <c r="BB7">
+        <f t="shared" si="2"/>
+        <v>5325.3871852700004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54">
       <c r="A8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8">
+        <v>523.26908582800002</v>
+      </c>
+      <c r="C8">
+        <v>2300</v>
+      </c>
+      <c r="D8">
+        <v>-3032.4333077900001</v>
+      </c>
+      <c r="E8">
+        <v>-655.33985219900001</v>
+      </c>
+      <c r="F8">
+        <v>-1922.204068</v>
+      </c>
+      <c r="G8">
+        <v>1644.0348199800001</v>
+      </c>
+      <c r="H8">
+        <v>-2140.7813110299999</v>
+      </c>
+      <c r="I8">
+        <v>-130.54579201499999</v>
+      </c>
+      <c r="J8">
+        <v>1208.9413163300001</v>
+      </c>
+      <c r="K8">
+        <v>2584.88248677</v>
+      </c>
+      <c r="L8">
+        <v>1623.56345334</v>
+      </c>
+      <c r="M8">
+        <v>850.385246327</v>
+      </c>
+      <c r="N8">
+        <v>1594.7384413699999</v>
+      </c>
+      <c r="O8">
+        <v>3170.74806932</v>
+      </c>
+      <c r="P8">
+        <v>1860.51103515</v>
+      </c>
+      <c r="Q8">
+        <v>3966.3322992600001</v>
+      </c>
+      <c r="R8">
+        <v>1300</v>
+      </c>
+      <c r="S8">
+        <v>1585.017985</v>
+      </c>
+      <c r="T8">
+        <v>765.91723285</v>
+      </c>
+      <c r="U8">
+        <v>383.988077277</v>
+      </c>
+      <c r="V8">
+        <v>-2372.1799320300001</v>
+      </c>
+      <c r="W8">
+        <v>-658.11158262599997</v>
+      </c>
+      <c r="X8">
+        <v>-1011.86557283</v>
+      </c>
+      <c r="Y8">
+        <v>-5397.8004698300001</v>
+      </c>
+      <c r="Z8">
+        <v>-2851.0140553199999</v>
+      </c>
+      <c r="AA8">
+        <v>206.345230421</v>
+      </c>
+      <c r="AB8">
+        <v>1233.3092335900001</v>
+      </c>
+      <c r="AC8">
+        <v>-1102.6173680700001</v>
+      </c>
+      <c r="AD8">
+        <v>1761.0039111999999</v>
+      </c>
+      <c r="AE8">
+        <v>2413.8329188900002</v>
+      </c>
+      <c r="AF8">
+        <v>-331.70555380600001</v>
+      </c>
+      <c r="AG8">
+        <v>1428.1493273399999</v>
+      </c>
+      <c r="AH8">
+        <v>2765.0576938999998</v>
+      </c>
+      <c r="AI8">
+        <v>605.06098457099995</v>
+      </c>
+      <c r="AJ8">
+        <v>2111.4210837099999</v>
+      </c>
+      <c r="AK8">
+        <v>-3336.9243387699998</v>
+      </c>
+      <c r="AL8">
+        <v>1243.6294370999999</v>
+      </c>
+      <c r="AM8">
+        <v>-90.153353233900006</v>
+      </c>
+      <c r="AN8">
+        <v>-463.03366281900003</v>
+      </c>
+      <c r="AO8">
+        <v>489.63800670400002</v>
+      </c>
+      <c r="AP8">
+        <v>2044.2983866100001</v>
+      </c>
+      <c r="AQ8">
+        <v>2305.4374360000002</v>
+      </c>
+      <c r="AR8">
+        <v>1209.9725554199999</v>
+      </c>
+      <c r="AS8">
+        <v>2449.6203150800002</v>
+      </c>
+      <c r="AT8">
+        <v>2166.5618715800001</v>
+      </c>
+      <c r="AU8">
+        <v>509.88767341300002</v>
+      </c>
+      <c r="AV8">
+        <v>-573.70467157500002</v>
+      </c>
+      <c r="AW8">
+        <v>-905.381689671</v>
+      </c>
+      <c r="AX8">
+        <v>-417.375765409</v>
+      </c>
+      <c r="AY8">
+        <v>915.95903442899998</v>
+      </c>
+      <c r="AZ8">
+        <f t="shared" si="0"/>
+        <v>476.56684603472212</v>
+      </c>
+      <c r="BA8">
+        <f t="shared" si="1"/>
+        <v>-5397.8004698300001</v>
+      </c>
+      <c r="BB8">
+        <f t="shared" si="2"/>
+        <v>3966.3322992600001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54">
       <c r="A9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9">
+        <v>359.755782114</v>
+      </c>
+      <c r="C9">
+        <v>304.02087992600002</v>
+      </c>
+      <c r="D9">
+        <v>1655.1500443899999</v>
+      </c>
+      <c r="E9">
+        <v>424.32497199099998</v>
+      </c>
+      <c r="F9">
+        <v>157.32006334600001</v>
+      </c>
+      <c r="G9">
+        <v>125.69820293799999</v>
+      </c>
+      <c r="H9">
+        <v>700.858034567</v>
+      </c>
+      <c r="I9">
+        <v>511.03906996799998</v>
+      </c>
+      <c r="J9">
+        <v>-109.535598366</v>
+      </c>
+      <c r="K9">
+        <v>-2653.62732383</v>
+      </c>
+      <c r="L9">
+        <v>-1382.8191629299999</v>
+      </c>
+      <c r="M9">
+        <v>-687.60160613599999</v>
+      </c>
+      <c r="N9">
+        <v>1045.3698945799999</v>
+      </c>
+      <c r="O9">
+        <v>-2598.7535859999998</v>
+      </c>
+      <c r="P9">
+        <v>500</v>
+      </c>
+      <c r="Q9">
+        <v>1345.57554723</v>
+      </c>
+      <c r="R9">
+        <v>322.38825675800001</v>
+      </c>
+      <c r="S9">
+        <v>1501.6361677</v>
+      </c>
+      <c r="T9">
+        <v>694.18061082400004</v>
+      </c>
+      <c r="U9">
+        <v>400.25552753800002</v>
+      </c>
+      <c r="V9">
+        <v>201.85555959300001</v>
+      </c>
+      <c r="W9">
+        <v>2300</v>
+      </c>
+      <c r="X9">
+        <v>2383.8726476299998</v>
+      </c>
+      <c r="Y9">
+        <v>767.61750468800005</v>
+      </c>
+      <c r="Z9">
+        <v>-31.836981442199999</v>
+      </c>
+      <c r="AA9">
+        <v>1754.39997965</v>
+      </c>
+      <c r="AB9">
+        <v>1050.7320107400001</v>
+      </c>
+      <c r="AC9">
+        <v>3500</v>
+      </c>
+      <c r="AD9">
+        <v>2300</v>
+      </c>
+      <c r="AE9">
+        <v>-381.19550783900002</v>
+      </c>
+      <c r="AF9">
+        <v>477.26505639700002</v>
+      </c>
+      <c r="AG9">
+        <v>-661.42276047899998</v>
+      </c>
+      <c r="AH9">
+        <v>1486.62499323</v>
+      </c>
+      <c r="AI9">
+        <v>1807.50537012</v>
+      </c>
+      <c r="AJ9">
+        <v>5130.4475942400004</v>
+      </c>
+      <c r="AK9">
+        <v>-673.97362291100001</v>
+      </c>
+      <c r="AL9">
+        <v>1428.8585815399999</v>
+      </c>
+      <c r="AM9">
+        <v>446.91855480499999</v>
+      </c>
+      <c r="AN9">
+        <v>1247.85100057</v>
+      </c>
+      <c r="AO9">
+        <v>1110.1588547599999</v>
+      </c>
+      <c r="AP9">
+        <v>2459.3012347600002</v>
+      </c>
+      <c r="AQ9">
+        <v>1203.08946094</v>
+      </c>
+      <c r="AR9">
+        <v>1522.49499997</v>
+      </c>
+      <c r="AS9">
+        <v>1547.22487729</v>
+      </c>
+      <c r="AT9">
+        <v>841.53404249300002</v>
+      </c>
+      <c r="AU9">
+        <v>1877.0705811299999</v>
+      </c>
+      <c r="AV9">
+        <v>1787.02313779</v>
+      </c>
+      <c r="AW9">
+        <v>399.54111970100001</v>
+      </c>
+      <c r="AX9">
+        <v>2546.1589515000001</v>
+      </c>
+      <c r="AY9">
+        <v>-676.20545301000004</v>
+      </c>
+      <c r="AZ9">
+        <f t="shared" si="0"/>
+        <v>835.36295128927611</v>
+      </c>
+      <c r="BA9">
+        <f t="shared" si="1"/>
+        <v>-2653.62732383</v>
+      </c>
+      <c r="BB9">
+        <f t="shared" si="2"/>
+        <v>5130.4475942400004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54">
       <c r="A10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="B10">
+        <v>1992.11089126</v>
+      </c>
+      <c r="C10">
+        <v>1638.93900403</v>
+      </c>
+      <c r="D10">
+        <v>1381.5780291799999</v>
+      </c>
+      <c r="E10">
+        <v>3109.8523921599999</v>
+      </c>
+      <c r="F10">
+        <v>-400.64478624100002</v>
+      </c>
+      <c r="G10">
+        <v>830.64149901300004</v>
+      </c>
+      <c r="H10">
+        <v>2853.8267423799998</v>
+      </c>
+      <c r="I10">
+        <v>738.59024254600001</v>
+      </c>
+      <c r="J10">
+        <v>217.09805616899999</v>
+      </c>
+      <c r="K10">
+        <v>336.30087258700001</v>
+      </c>
+      <c r="L10">
+        <v>1976.4588486800001</v>
+      </c>
+      <c r="M10">
+        <v>773.77683346399999</v>
+      </c>
+      <c r="N10">
+        <v>1315.3552526799999</v>
+      </c>
+      <c r="O10">
+        <v>1942.7695853499999</v>
+      </c>
+      <c r="P10">
+        <v>-1851.2049704599999</v>
+      </c>
+      <c r="Q10">
+        <v>758.46202915399999</v>
+      </c>
+      <c r="R10">
+        <v>-356.38696462000001</v>
+      </c>
+      <c r="S10">
+        <v>1853.19454172</v>
+      </c>
+      <c r="T10">
+        <v>-2722.0403434499999</v>
+      </c>
+      <c r="U10">
+        <v>3151.4393517799999</v>
+      </c>
+      <c r="V10">
+        <v>1715.66784966</v>
+      </c>
+      <c r="W10">
+        <v>1085.26487077</v>
+      </c>
+      <c r="X10">
+        <v>1180.29273833</v>
+      </c>
+      <c r="Y10">
+        <v>1964.34204675</v>
+      </c>
+      <c r="Z10">
+        <v>476.55645335299999</v>
+      </c>
+      <c r="AA10">
+        <v>1583.02041325</v>
+      </c>
+      <c r="AB10">
+        <v>2279.4982420400002</v>
+      </c>
+      <c r="AC10">
+        <v>826.34534187700001</v>
+      </c>
+      <c r="AD10">
+        <v>3895.1645643299998</v>
+      </c>
+      <c r="AE10">
+        <v>908.37182452100001</v>
+      </c>
+      <c r="AF10">
+        <v>1214.3087131499999</v>
+      </c>
+      <c r="AG10">
+        <v>2902.29584961</v>
+      </c>
+      <c r="AH10">
+        <v>-731.63770607200001</v>
+      </c>
+      <c r="AI10">
+        <v>306.77443242099997</v>
+      </c>
+      <c r="AJ10">
+        <v>1299.4080102800001</v>
+      </c>
+      <c r="AK10">
+        <v>1487.8595293599999</v>
+      </c>
+      <c r="AL10">
+        <v>-1132.1620104900001</v>
+      </c>
+      <c r="AM10">
+        <v>-1377.9585949499999</v>
+      </c>
+      <c r="AN10">
+        <v>492.978620885</v>
+      </c>
+      <c r="AO10">
+        <v>-746.60094935400002</v>
+      </c>
+      <c r="AP10">
+        <v>746.67249852899999</v>
+      </c>
+      <c r="AQ10">
+        <v>2085.4813825800002</v>
+      </c>
+      <c r="AR10">
+        <v>-3207.1826806099998</v>
+      </c>
+      <c r="AS10">
+        <v>-260.270807053</v>
+      </c>
+      <c r="AT10">
+        <v>-254.847933192</v>
+      </c>
+      <c r="AU10">
+        <v>2754.19383023</v>
+      </c>
+      <c r="AV10">
+        <v>1456.0189559</v>
+      </c>
+      <c r="AW10">
+        <v>803.91103814300004</v>
+      </c>
+      <c r="AX10">
+        <v>1175.2318821700001</v>
+      </c>
+      <c r="AY10">
+        <v>634.25778580799999</v>
+      </c>
+      <c r="AZ10">
+        <f t="shared" si="0"/>
+        <v>902.06746599216001</v>
+      </c>
+      <c r="BA10">
+        <f t="shared" si="1"/>
+        <v>-3207.1826806099998</v>
+      </c>
+      <c r="BB10">
+        <f t="shared" si="2"/>
+        <v>3895.1645643299998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54">
       <c r="A11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="B11">
+        <v>784.66959527300003</v>
+      </c>
+      <c r="C11">
+        <v>1837.75969917</v>
+      </c>
+      <c r="D11">
+        <v>1173.5549000599999</v>
+      </c>
+      <c r="E11">
+        <v>2204.6484439800001</v>
+      </c>
+      <c r="F11">
+        <v>1128.60675601</v>
+      </c>
+      <c r="G11">
+        <v>3842.21465382</v>
+      </c>
+      <c r="H11">
+        <v>2516.5055478700001</v>
+      </c>
+      <c r="I11">
+        <v>1858.44904099</v>
+      </c>
+      <c r="J11">
+        <v>1778.5085708300001</v>
+      </c>
+      <c r="K11">
+        <v>1506.01344632</v>
+      </c>
+      <c r="L11">
+        <v>1678.2049297399999</v>
+      </c>
+      <c r="M11">
+        <v>968.85309461999998</v>
+      </c>
+      <c r="N11">
+        <v>2980.1849461000002</v>
+      </c>
+      <c r="O11">
+        <v>-2540.2256264299999</v>
+      </c>
+      <c r="P11">
+        <v>813.59809259600001</v>
+      </c>
+      <c r="Q11">
+        <v>323.35229720199999</v>
+      </c>
+      <c r="R11">
+        <v>973.79062870500002</v>
+      </c>
+      <c r="S11">
+        <v>1131.9531877700001</v>
+      </c>
+      <c r="T11">
+        <v>1245.6071257399999</v>
+      </c>
+      <c r="U11">
+        <v>990.33896140800005</v>
+      </c>
+      <c r="V11">
+        <v>548.21481850500004</v>
+      </c>
+      <c r="W11">
+        <v>1943.17799307</v>
+      </c>
+      <c r="X11">
+        <v>4700</v>
+      </c>
+      <c r="Y11">
+        <v>1661.3600970699999</v>
+      </c>
+      <c r="Z11">
+        <v>2147.5043811199998</v>
+      </c>
+      <c r="AA11">
+        <v>1957.6982032000001</v>
+      </c>
+      <c r="AB11">
+        <v>956.618826023</v>
+      </c>
+      <c r="AC11">
+        <v>-333.67428189200001</v>
+      </c>
+      <c r="AD11">
+        <v>-2233.1502199199999</v>
+      </c>
+      <c r="AE11">
+        <v>2323.09637101</v>
+      </c>
+      <c r="AF11">
+        <v>1173.1870770800001</v>
+      </c>
+      <c r="AG11">
+        <v>-1552.03748118</v>
+      </c>
+      <c r="AH11">
+        <v>485.509129433</v>
+      </c>
+      <c r="AI11">
+        <v>1077.64586403</v>
+      </c>
+      <c r="AJ11">
+        <v>375.00675265299998</v>
+      </c>
+      <c r="AK11">
+        <v>1433.3866697599999</v>
+      </c>
+      <c r="AL11">
+        <v>2254.0451836799998</v>
+      </c>
+      <c r="AM11">
+        <v>37.229737023399998</v>
+      </c>
+      <c r="AN11">
+        <v>1626.67269414</v>
+      </c>
+      <c r="AO11">
+        <v>2097.2478151</v>
+      </c>
+      <c r="AP11">
+        <v>2070.0736109099998</v>
+      </c>
+      <c r="AQ11">
+        <v>1634.8563159600001</v>
+      </c>
+      <c r="AR11">
+        <v>2404.7132569300002</v>
+      </c>
+      <c r="AS11">
+        <v>-1593.25940023</v>
+      </c>
+      <c r="AT11">
+        <v>466.55644005099998</v>
+      </c>
+      <c r="AU11">
+        <v>1386.5252122300001</v>
+      </c>
+      <c r="AV11">
+        <v>-611.03717743499999</v>
+      </c>
+      <c r="AW11">
+        <v>2486.6408071199999</v>
+      </c>
+      <c r="AX11">
+        <v>1935.44516477</v>
+      </c>
+      <c r="AY11">
+        <v>1696.42982532</v>
+      </c>
+      <c r="AZ11">
+        <f t="shared" si="0"/>
+        <v>1235.0454395461077</v>
+      </c>
+      <c r="BA11">
+        <f t="shared" si="1"/>
+        <v>-2540.2256264299999</v>
+      </c>
+      <c r="BB11">
+        <f t="shared" si="2"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54">
       <c r="A12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="B12">
+        <v>1467.4652363099999</v>
+      </c>
+      <c r="C12">
+        <v>-3588.9113287999999</v>
+      </c>
+      <c r="D12">
+        <v>-4433.9696377299997</v>
+      </c>
+      <c r="E12">
+        <v>1885.08745006</v>
+      </c>
+      <c r="F12">
+        <v>837.69534716199996</v>
+      </c>
+      <c r="G12">
+        <v>-639.18280444599998</v>
+      </c>
+      <c r="H12">
+        <v>2691.45885692</v>
+      </c>
+      <c r="I12">
+        <v>1139.9971557700001</v>
+      </c>
+      <c r="J12">
+        <v>-2290.1690263400001</v>
+      </c>
+      <c r="K12">
+        <v>4062.9270797499998</v>
+      </c>
+      <c r="L12">
+        <v>3259.7056535199999</v>
+      </c>
+      <c r="M12">
+        <v>3626.0449739599999</v>
+      </c>
+      <c r="N12">
+        <v>-441.02692560999998</v>
+      </c>
+      <c r="O12">
+        <v>735.77304687599997</v>
+      </c>
+      <c r="P12">
+        <v>2338.0823483300001</v>
+      </c>
+      <c r="Q12">
+        <v>116.908835431</v>
+      </c>
+      <c r="R12">
+        <v>1584.8186110700001</v>
+      </c>
+      <c r="S12">
+        <v>2784.2822215800002</v>
+      </c>
+      <c r="T12">
+        <v>2986.0739953699999</v>
+      </c>
+      <c r="U12">
+        <v>1262.1548063499999</v>
+      </c>
+      <c r="V12">
+        <v>-1564.0804247599999</v>
+      </c>
+      <c r="W12">
+        <v>1206.7382262399999</v>
+      </c>
+      <c r="X12">
+        <v>1520.85823583</v>
+      </c>
+      <c r="Y12">
+        <v>1670.94963768</v>
+      </c>
+      <c r="Z12">
+        <v>769.02220485500004</v>
+      </c>
+      <c r="AA12">
+        <v>847.30522337599996</v>
+      </c>
+      <c r="AB12">
+        <v>600.32505424700003</v>
+      </c>
+      <c r="AC12">
+        <v>1174.1751841600001</v>
+      </c>
+      <c r="AD12">
+        <v>1010.21884471</v>
+      </c>
+      <c r="AE12">
+        <v>2999.57072659</v>
+      </c>
+      <c r="AF12">
+        <v>2592.38770075</v>
+      </c>
+      <c r="AG12">
+        <v>93.178338549299994</v>
+      </c>
+      <c r="AH12">
+        <v>3312.1668346000001</v>
+      </c>
+      <c r="AI12">
+        <v>-5240.2722557999996</v>
+      </c>
+      <c r="AJ12">
+        <v>1440.3258226400001</v>
+      </c>
+      <c r="AK12">
+        <v>1554.09288373</v>
+      </c>
+      <c r="AL12">
+        <v>-430.014575724</v>
+      </c>
+      <c r="AM12">
+        <v>-677.28612384300004</v>
+      </c>
+      <c r="AN12">
+        <v>3851.4210201400001</v>
+      </c>
+      <c r="AO12">
+        <v>208.036091621</v>
+      </c>
+      <c r="AP12">
+        <v>2113.14703005</v>
+      </c>
+      <c r="AQ12">
+        <v>-1758.22497774</v>
+      </c>
+      <c r="AR12">
+        <v>754.08330204799995</v>
+      </c>
+      <c r="AS12">
+        <v>2647.2238546899998</v>
+      </c>
+      <c r="AT12">
+        <v>2685.5665193</v>
+      </c>
+      <c r="AU12">
+        <v>-20.023545350399999</v>
+      </c>
+      <c r="AV12">
+        <v>1713.63432532</v>
+      </c>
+      <c r="AW12">
+        <v>-276.95448697699999</v>
+      </c>
+      <c r="AX12">
+        <v>-1531.92395087</v>
+      </c>
+      <c r="AY12">
+        <v>1632.7797467600001</v>
+      </c>
+      <c r="AZ12">
+        <f t="shared" si="0"/>
+        <v>885.67284724709816</v>
+      </c>
+      <c r="BA12">
+        <f t="shared" si="1"/>
+        <v>-5240.2722557999996</v>
+      </c>
+      <c r="BB12">
+        <f t="shared" si="2"/>
+        <v>4062.9270797499998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54">
       <c r="A13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13">
+        <v>964.60739346599996</v>
+      </c>
+      <c r="C13">
+        <v>744.37236639100001</v>
+      </c>
+      <c r="D13">
+        <v>528.77147265500003</v>
+      </c>
+      <c r="E13">
+        <v>959.98862474299995</v>
+      </c>
+      <c r="F13">
+        <v>1095.8082345400001</v>
+      </c>
+      <c r="G13">
+        <v>-658.65371382399996</v>
+      </c>
+      <c r="H13">
+        <v>640.39265211300005</v>
+      </c>
+      <c r="I13">
+        <v>2929.9234568500001</v>
+      </c>
+      <c r="J13">
+        <v>793.80578559699995</v>
+      </c>
+      <c r="K13">
+        <v>445.06226979399997</v>
+      </c>
+      <c r="L13">
+        <v>1098.0779271599999</v>
+      </c>
+      <c r="M13">
+        <v>1322.0696258</v>
+      </c>
+      <c r="N13">
+        <v>402.52780469599998</v>
+      </c>
+      <c r="O13">
+        <v>440.70522404100001</v>
+      </c>
+      <c r="P13">
+        <v>928.12570997600005</v>
+      </c>
+      <c r="Q13">
+        <v>100</v>
+      </c>
+      <c r="R13">
+        <v>630.13095772600002</v>
+      </c>
+      <c r="S13">
+        <v>306.67357598299998</v>
+      </c>
+      <c r="T13">
+        <v>926.37203113500004</v>
+      </c>
+      <c r="U13">
+        <v>1760.90762094</v>
+      </c>
+      <c r="V13">
+        <v>2619.7569582599999</v>
+      </c>
+      <c r="W13">
+        <v>-3332.3117143899999</v>
+      </c>
+      <c r="X13">
+        <v>1003.71511465</v>
+      </c>
+      <c r="Y13">
+        <v>-2100</v>
+      </c>
+      <c r="Z13">
+        <v>-5539.7291156900001</v>
+      </c>
+      <c r="AA13">
+        <v>-198.604483437</v>
+      </c>
+      <c r="AB13">
+        <v>628.94569578699998</v>
+      </c>
+      <c r="AC13">
+        <v>-6063.4669799200001</v>
+      </c>
+      <c r="AD13">
+        <v>158.17022782500001</v>
+      </c>
+      <c r="AE13">
+        <v>404.014028166</v>
+      </c>
+      <c r="AF13">
+        <v>3130.6622465099999</v>
+      </c>
+      <c r="AG13">
+        <v>983.51567231499996</v>
+      </c>
+      <c r="AH13">
+        <v>1269.4315145400001</v>
+      </c>
+      <c r="AI13">
+        <v>733.67794317300002</v>
+      </c>
+      <c r="AJ13">
+        <v>-1317.5593386099999</v>
+      </c>
+      <c r="AK13">
+        <v>2881.1575053299998</v>
+      </c>
+      <c r="AL13">
+        <v>1055.0600972499999</v>
+      </c>
+      <c r="AM13">
+        <v>639.19506970899999</v>
+      </c>
+      <c r="AN13">
+        <v>1042.0423198599999</v>
+      </c>
+      <c r="AO13">
+        <v>-2408.2942068900002</v>
+      </c>
+      <c r="AP13">
+        <v>322.59137176299998</v>
+      </c>
+      <c r="AQ13">
+        <v>-1340.16976144</v>
+      </c>
+      <c r="AR13">
+        <v>71.211773195399999</v>
+      </c>
+      <c r="AS13">
+        <v>1606.0614061700001</v>
+      </c>
+      <c r="AT13">
+        <v>2752.81716026</v>
+      </c>
+      <c r="AU13">
+        <v>909.71720914599996</v>
+      </c>
+      <c r="AV13">
+        <v>-339.39333656899998</v>
+      </c>
+      <c r="AW13">
+        <v>2483.03002612</v>
+      </c>
+      <c r="AX13">
+        <v>1689.4429750100001</v>
+      </c>
+      <c r="AY13">
+        <v>3751.5658674000001</v>
+      </c>
+      <c r="AZ13">
+        <f t="shared" si="0"/>
+        <v>477.11844530550798</v>
+      </c>
+      <c r="BA13">
+        <f t="shared" si="1"/>
+        <v>-6063.4669799200001</v>
+      </c>
+      <c r="BB13">
+        <f t="shared" si="2"/>
+        <v>3751.5658674000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54">
       <c r="A14">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="B14">
+        <v>582.80538161300001</v>
+      </c>
+      <c r="C14">
+        <v>1706.81992691</v>
+      </c>
+      <c r="D14">
+        <v>1078.99404736</v>
+      </c>
+      <c r="E14">
+        <v>1897.1415066300001</v>
+      </c>
+      <c r="F14">
+        <v>428.31169213499999</v>
+      </c>
+      <c r="G14">
+        <v>1090.1106683400001</v>
+      </c>
+      <c r="H14">
+        <v>6957.65347759</v>
+      </c>
+      <c r="I14">
+        <v>2405.8279939899999</v>
+      </c>
+      <c r="J14">
+        <v>588.35867260800001</v>
+      </c>
+      <c r="K14">
+        <v>-250.39631576599999</v>
+      </c>
+      <c r="L14">
+        <v>4653.9732842100002</v>
+      </c>
+      <c r="M14">
+        <v>-748.50257617800003</v>
+      </c>
+      <c r="N14">
+        <v>1692.1998641499999</v>
+      </c>
+      <c r="O14">
+        <v>2424.7012076199999</v>
+      </c>
+      <c r="P14">
+        <v>1844.53720645</v>
+      </c>
+      <c r="Q14">
+        <v>1861.8343108199999</v>
+      </c>
+      <c r="R14">
+        <v>1023.69082793</v>
+      </c>
+      <c r="S14">
+        <v>676.511953619</v>
+      </c>
+      <c r="T14">
+        <v>5172.1205464900004</v>
+      </c>
+      <c r="U14">
+        <v>806.63482818900002</v>
+      </c>
+      <c r="V14">
+        <v>1939.98029185</v>
+      </c>
+      <c r="W14">
+        <v>3203.9695666500002</v>
+      </c>
+      <c r="X14">
+        <v>1266.2587496399999</v>
+      </c>
+      <c r="Y14">
+        <v>2081.7578442600002</v>
+      </c>
+      <c r="Z14">
+        <v>7438.0657553600004</v>
+      </c>
+      <c r="AA14">
+        <v>1671.6249932799999</v>
+      </c>
+      <c r="AB14">
+        <v>-515.42594904500004</v>
+      </c>
+      <c r="AC14">
+        <v>3494.3278154099999</v>
+      </c>
+      <c r="AD14">
+        <v>468.68144919100001</v>
+      </c>
+      <c r="AE14">
+        <v>1796.31552702</v>
+      </c>
+      <c r="AF14">
+        <v>651.03116473600005</v>
+      </c>
+      <c r="AG14">
+        <v>255.23941375800001</v>
+      </c>
+      <c r="AH14">
+        <v>-1983.22426275</v>
+      </c>
+      <c r="AI14">
+        <v>862.82951496400005</v>
+      </c>
+      <c r="AJ14">
+        <v>2785.8583646400002</v>
+      </c>
+      <c r="AK14">
+        <v>1273.3595226800001</v>
+      </c>
+      <c r="AL14">
+        <v>2694.9823678299999</v>
+      </c>
+      <c r="AM14">
+        <v>399.83104043200001</v>
+      </c>
+      <c r="AN14">
+        <v>1208.78379365</v>
+      </c>
+      <c r="AO14">
+        <v>3774.64106554</v>
+      </c>
+      <c r="AP14">
+        <v>3973.88194634</v>
+      </c>
+      <c r="AQ14">
+        <v>1405.8787158</v>
+      </c>
+      <c r="AR14">
+        <v>3439.2727608</v>
+      </c>
+      <c r="AS14">
+        <v>1423.9614669699999</v>
+      </c>
+      <c r="AT14">
+        <v>3329.5655900500001</v>
+      </c>
+      <c r="AU14">
+        <v>-500.42879479999999</v>
+      </c>
+      <c r="AV14">
+        <v>1271.4369197799999</v>
+      </c>
+      <c r="AW14">
+        <v>-2402.2915102699999</v>
+      </c>
+      <c r="AX14">
+        <v>2216.46228096</v>
+      </c>
+      <c r="AY14">
+        <v>292.17589311299997</v>
+      </c>
+      <c r="AZ14">
+        <f t="shared" si="0"/>
+        <v>1702.2426360509794</v>
+      </c>
+      <c r="BA14">
+        <f t="shared" si="1"/>
+        <v>-2402.2915102699999</v>
+      </c>
+      <c r="BB14">
+        <f t="shared" si="2"/>
+        <v>7438.0657553600004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54">
       <c r="A15">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="B15">
+        <v>-436.36431682199998</v>
+      </c>
+      <c r="C15">
+        <v>3049.2527608</v>
+      </c>
+      <c r="D15">
+        <v>89.856485947600007</v>
+      </c>
+      <c r="E15">
+        <v>1733.8696572900001</v>
+      </c>
+      <c r="F15">
+        <v>3577.71227589</v>
+      </c>
+      <c r="G15">
+        <v>-342.29350672700002</v>
+      </c>
+      <c r="H15">
+        <v>6180.8689637799998</v>
+      </c>
+      <c r="I15">
+        <v>1560.18174662</v>
+      </c>
+      <c r="J15">
+        <v>-1216.09648137</v>
+      </c>
+      <c r="K15">
+        <v>2072.9100077799999</v>
+      </c>
+      <c r="L15">
+        <v>3480.08632025</v>
+      </c>
+      <c r="M15">
+        <v>1924.7630706499999</v>
+      </c>
+      <c r="N15">
+        <v>-3686.0006866399999</v>
+      </c>
+      <c r="O15">
+        <v>1166.76882907</v>
+      </c>
+      <c r="P15">
+        <v>6133.17510029</v>
+      </c>
+      <c r="Q15">
+        <v>1775.0814908499999</v>
+      </c>
+      <c r="R15">
+        <v>471.44919585999997</v>
+      </c>
+      <c r="S15">
+        <v>982.43761550299996</v>
+      </c>
+      <c r="T15">
+        <v>3232.1125417500002</v>
+      </c>
+      <c r="U15">
+        <v>3238.6453203999999</v>
+      </c>
+      <c r="V15">
+        <v>2081.8244928499998</v>
+      </c>
+      <c r="W15">
+        <v>-31.571218358900001</v>
+      </c>
+      <c r="X15">
+        <v>1136.7680545999999</v>
+      </c>
+      <c r="Y15">
+        <v>1229.7550004100001</v>
+      </c>
+      <c r="Z15">
+        <v>2970.5636729399998</v>
+      </c>
+      <c r="AA15">
+        <v>-54.3813864245</v>
+      </c>
+      <c r="AB15">
+        <v>-900.144493216</v>
+      </c>
+      <c r="AC15">
+        <v>208.472452465</v>
+      </c>
+      <c r="AD15">
+        <v>-2318.3721991100001</v>
+      </c>
+      <c r="AE15">
+        <v>613.43409998300001</v>
+      </c>
+      <c r="AF15">
+        <v>-615.91903062999995</v>
+      </c>
+      <c r="AG15">
+        <v>2433.01265646</v>
+      </c>
+      <c r="AH15">
+        <v>2050.0700998699999</v>
+      </c>
+      <c r="AI15">
+        <v>-2810.5806008</v>
+      </c>
+      <c r="AJ15">
+        <v>-388.47784021799998</v>
+      </c>
+      <c r="AK15">
+        <v>1251.3720228</v>
+      </c>
+      <c r="AL15">
+        <v>-1414.4211273000001</v>
+      </c>
+      <c r="AM15">
+        <v>-640.47462150700005</v>
+      </c>
+      <c r="AN15">
+        <v>816.57537085599995</v>
+      </c>
+      <c r="AO15">
+        <v>1095.5466295199999</v>
+      </c>
+      <c r="AP15">
+        <v>1807.7001516400001</v>
+      </c>
+      <c r="AQ15">
+        <v>-6963.8332301399996</v>
+      </c>
+      <c r="AR15">
+        <v>-5152.51779455</v>
+      </c>
+      <c r="AS15">
+        <v>586.60924030599995</v>
+      </c>
+      <c r="AT15">
+        <v>542.30315475800001</v>
+      </c>
+      <c r="AU15">
+        <v>3286.7379691299998</v>
+      </c>
+      <c r="AV15">
+        <v>-1755.75712561</v>
+      </c>
+      <c r="AW15">
+        <v>210.333162098</v>
+      </c>
+      <c r="AX15">
+        <v>1015.97485493</v>
+      </c>
+      <c r="AY15">
+        <v>368.07416001399997</v>
+      </c>
+      <c r="AZ15">
+        <f t="shared" si="0"/>
+        <v>712.94185937874397</v>
+      </c>
+      <c r="BA15">
+        <f t="shared" si="1"/>
+        <v>-6963.8332301399996</v>
+      </c>
+      <c r="BB15">
+        <f t="shared" si="2"/>
+        <v>6180.8689637799998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54">
       <c r="A16">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>947.20032853700002</v>
+      </c>
+      <c r="C16">
+        <v>1786.86936165</v>
+      </c>
+      <c r="D16">
+        <v>812.48143690500001</v>
+      </c>
+      <c r="E16">
+        <v>4038.2420533700001</v>
+      </c>
+      <c r="F16">
+        <v>888.53882337799996</v>
+      </c>
+      <c r="G16">
+        <v>1964.15692969</v>
+      </c>
+      <c r="H16">
+        <v>1797.1797799599999</v>
+      </c>
+      <c r="I16">
+        <v>1088.24424778</v>
+      </c>
+      <c r="J16">
+        <v>2202.9355953499999</v>
+      </c>
+      <c r="K16">
+        <v>458.18131888200003</v>
+      </c>
+      <c r="L16">
+        <v>785.89214727299998</v>
+      </c>
+      <c r="M16">
+        <v>621.22143162199995</v>
+      </c>
+      <c r="N16">
+        <v>958.05859998999995</v>
+      </c>
+      <c r="O16">
+        <v>333.90582104700002</v>
+      </c>
+      <c r="P16">
+        <v>2319.34698669</v>
+      </c>
+      <c r="Q16">
+        <v>1492.4336819800001</v>
+      </c>
+      <c r="R16">
+        <v>1687.75339796</v>
+      </c>
+      <c r="S16">
+        <v>1876.7975063900001</v>
+      </c>
+      <c r="T16">
+        <v>35.094169860800001</v>
+      </c>
+      <c r="U16">
+        <v>100.22501192999999</v>
+      </c>
+      <c r="V16">
+        <v>-234.514601511</v>
+      </c>
+      <c r="W16">
+        <v>1094.1926371</v>
+      </c>
+      <c r="X16">
+        <v>168.76351016199999</v>
+      </c>
+      <c r="Y16">
+        <v>1927.3789643299999</v>
+      </c>
+      <c r="Z16">
+        <v>3563.96138883</v>
+      </c>
+      <c r="AA16">
+        <v>2466.2434224600001</v>
+      </c>
+      <c r="AB16">
+        <v>-1728.35249632</v>
+      </c>
+      <c r="AC16">
+        <v>329.35119399500002</v>
+      </c>
+      <c r="AD16">
+        <v>1619.4030443500001</v>
+      </c>
+      <c r="AE16">
+        <v>2869.86395017</v>
+      </c>
+      <c r="AF16">
+        <v>1288.4695097399999</v>
+      </c>
+      <c r="AG16">
+        <v>987.47488389900002</v>
+      </c>
+      <c r="AH16">
+        <v>4520.5483167499997</v>
+      </c>
+      <c r="AI16">
+        <v>1931.9499516799999</v>
+      </c>
+      <c r="AJ16">
+        <v>1564.2255514799999</v>
+      </c>
+      <c r="AK16">
+        <v>844.11925176499994</v>
+      </c>
+      <c r="AL16">
+        <v>-1735.5496792500001</v>
+      </c>
+      <c r="AM16">
+        <v>288.662657293</v>
+      </c>
+      <c r="AN16">
+        <v>781.94465750899997</v>
+      </c>
+      <c r="AO16">
+        <v>-2280.2401986999998</v>
+      </c>
+      <c r="AP16">
+        <v>1601.4822103199999</v>
+      </c>
+      <c r="AQ16">
+        <v>1410.69791538</v>
+      </c>
+      <c r="AR16">
+        <v>-1347.5573264699999</v>
+      </c>
+      <c r="AS16">
+        <v>1430.1305928100001</v>
+      </c>
+      <c r="AT16">
+        <v>-482.73749230300001</v>
+      </c>
+      <c r="AU16">
+        <v>1299.35800961</v>
+      </c>
+      <c r="AV16">
+        <v>10.114250284100001</v>
+      </c>
+      <c r="AW16">
+        <v>703.24497886799998</v>
+      </c>
+      <c r="AX16">
+        <v>-1986.6079209</v>
+      </c>
+      <c r="AY16">
+        <v>-343.758739875</v>
+      </c>
+      <c r="AZ16">
+        <f t="shared" si="0"/>
+        <v>975.14042047401801</v>
+      </c>
+      <c r="BA16">
+        <f t="shared" si="1"/>
+        <v>-2280.2401986999998</v>
+      </c>
+      <c r="BB16">
+        <f t="shared" si="2"/>
+        <v>4520.5483167499997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:54">
       <c r="A17">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>554.33729768800004</v>
+      </c>
+      <c r="C17">
+        <v>918.47396763200004</v>
+      </c>
+      <c r="D17">
+        <v>755.62545616099999</v>
+      </c>
+      <c r="E17">
+        <v>1595.3346905999999</v>
+      </c>
+      <c r="F17">
+        <v>2670.3133109</v>
+      </c>
+      <c r="G17">
+        <v>2637.5647210400002</v>
+      </c>
+      <c r="H17">
+        <v>-2497.2788206300002</v>
+      </c>
+      <c r="I17">
+        <v>1166.1957950399999</v>
+      </c>
+      <c r="J17">
+        <v>-1672.05531002</v>
+      </c>
+      <c r="K17">
+        <v>-186.299027884</v>
+      </c>
+      <c r="L17">
+        <v>-1501.38975327</v>
+      </c>
+      <c r="M17">
+        <v>1908.1353697</v>
+      </c>
+      <c r="N17">
+        <v>711.34418166900002</v>
+      </c>
+      <c r="O17">
+        <v>510.921364127</v>
+      </c>
+      <c r="P17">
+        <v>1347.14089448</v>
+      </c>
+      <c r="Q17">
+        <v>1084.9938429199999</v>
+      </c>
+      <c r="R17">
+        <v>1521.1919529500001</v>
+      </c>
+      <c r="S17">
+        <v>-313.92286626700002</v>
+      </c>
+      <c r="T17">
+        <v>885.62144507999994</v>
+      </c>
+      <c r="U17">
+        <v>1410.37753578</v>
+      </c>
+      <c r="V17">
+        <v>1785.0690720299999</v>
+      </c>
+      <c r="W17">
+        <v>641.73812640400001</v>
+      </c>
+      <c r="X17">
+        <v>388.69452982600001</v>
+      </c>
+      <c r="Y17">
+        <v>2547.0172828999998</v>
+      </c>
+      <c r="Z17">
+        <v>1978.16911927</v>
+      </c>
+      <c r="AA17">
+        <v>-574.90150554599995</v>
+      </c>
+      <c r="AB17">
+        <v>1385.7842192600001</v>
+      </c>
+      <c r="AC17">
+        <v>1040.7623822999999</v>
+      </c>
+      <c r="AD17">
+        <v>745.49769789699997</v>
+      </c>
+      <c r="AE17">
+        <v>716.30413125899997</v>
+      </c>
+      <c r="AF17">
+        <v>894.69993872099997</v>
+      </c>
+      <c r="AG17">
+        <v>655.90024469100001</v>
+      </c>
+      <c r="AH17">
+        <v>682.41485077699997</v>
+      </c>
+      <c r="AI17">
+        <v>3734.2967049399999</v>
+      </c>
+      <c r="AJ17">
+        <v>1597.41180405</v>
+      </c>
+      <c r="AK17">
+        <v>1297.0858151800001</v>
+      </c>
+      <c r="AL17">
+        <v>993.47597970699996</v>
+      </c>
+      <c r="AM17">
+        <v>518.91576696000004</v>
+      </c>
+      <c r="AN17">
+        <v>1641.1928972799999</v>
+      </c>
+      <c r="AO17">
+        <v>-426.61463900000001</v>
+      </c>
+      <c r="AP17">
+        <v>1655.32702322</v>
+      </c>
+      <c r="AQ17">
+        <v>276.142262652</v>
+      </c>
+      <c r="AR17">
+        <v>1397.4848629999999</v>
+      </c>
+      <c r="AS17">
+        <v>672.66503301</v>
+      </c>
+      <c r="AT17">
+        <v>1885.6000582199999</v>
+      </c>
+      <c r="AU17">
+        <v>-768.06199950099995</v>
+      </c>
+      <c r="AV17">
+        <v>969.66467288700005</v>
+      </c>
+      <c r="AW17">
+        <v>46.013988443199999</v>
+      </c>
+      <c r="AX17">
+        <v>310.07546559299999</v>
+      </c>
+      <c r="AY17">
+        <v>4385.4647864999997</v>
+      </c>
+      <c r="AZ17">
+        <f t="shared" si="0"/>
+        <v>931.5983324125242</v>
+      </c>
+      <c r="BA17">
+        <f t="shared" si="1"/>
+        <v>-2497.2788206300002</v>
+      </c>
+      <c r="BB17">
+        <f t="shared" si="2"/>
+        <v>4385.4647864999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:54">
       <c r="A18">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>476.12655513200002</v>
+      </c>
+      <c r="C18">
+        <v>2832.2038177999998</v>
+      </c>
+      <c r="D18">
+        <v>978.89592206099996</v>
+      </c>
+      <c r="E18">
+        <v>4552.47847525</v>
+      </c>
+      <c r="F18">
+        <v>702.78369800400003</v>
+      </c>
+      <c r="G18">
+        <v>-2369.1117531899999</v>
+      </c>
+      <c r="H18">
+        <v>1693.32918503</v>
+      </c>
+      <c r="I18">
+        <v>1745.8814803600001</v>
+      </c>
+      <c r="J18">
+        <v>2768.69710846</v>
+      </c>
+      <c r="K18">
+        <v>3237.4747508199998</v>
+      </c>
+      <c r="L18">
+        <v>327.02674179000002</v>
+      </c>
+      <c r="M18">
+        <v>3850.5985464999999</v>
+      </c>
+      <c r="N18">
+        <v>1718.75490236</v>
+      </c>
+      <c r="O18">
+        <v>2367.1528556899998</v>
+      </c>
+      <c r="P18">
+        <v>3813.1547312299999</v>
+      </c>
+      <c r="Q18">
+        <v>1325.2498401600001</v>
+      </c>
+      <c r="R18">
+        <v>833.68274003099998</v>
+      </c>
+      <c r="S18">
+        <v>1893.26885382</v>
+      </c>
+      <c r="T18">
+        <v>-6182.6028599499996</v>
+      </c>
+      <c r="U18">
+        <v>-1409.68371785</v>
+      </c>
+      <c r="V18">
+        <v>141.42376349200001</v>
+      </c>
+      <c r="W18">
+        <v>2907.0500350500001</v>
+      </c>
+      <c r="X18">
+        <v>-571.14258636800002</v>
+      </c>
+      <c r="Y18">
+        <v>3375.8945093900002</v>
+      </c>
+      <c r="Z18">
+        <v>3910.2120896199999</v>
+      </c>
+      <c r="AA18">
+        <v>3760.7105057399999</v>
+      </c>
+      <c r="AB18">
+        <v>3164.7717803999999</v>
+      </c>
+      <c r="AC18">
+        <v>-1127.43000736</v>
+      </c>
+      <c r="AD18">
+        <v>992.15080704900004</v>
+      </c>
+      <c r="AE18">
+        <v>-3416.4218094799999</v>
+      </c>
+      <c r="AF18">
+        <v>-824.19305285099995</v>
+      </c>
+      <c r="AG18">
+        <v>3346.0624939899999</v>
+      </c>
+      <c r="AH18">
+        <v>729.92693703500004</v>
+      </c>
+      <c r="AI18">
+        <v>-2547.9912335499998</v>
+      </c>
+      <c r="AJ18">
+        <v>2250.80058138</v>
+      </c>
+      <c r="AK18">
+        <v>3083.3068128199998</v>
+      </c>
+      <c r="AL18">
+        <v>6067.9239335299999</v>
+      </c>
+      <c r="AM18">
+        <v>1225.3473368099999</v>
+      </c>
+      <c r="AN18">
+        <v>693.13376799000002</v>
+      </c>
+      <c r="AO18">
+        <v>332.17275195299999</v>
+      </c>
+      <c r="AP18">
+        <v>305.15062344</v>
+      </c>
+      <c r="AQ18">
+        <v>4179.9604110999999</v>
+      </c>
+      <c r="AR18">
+        <v>427.545944491</v>
+      </c>
+      <c r="AS18">
+        <v>2699.6077659699999</v>
+      </c>
+      <c r="AT18">
+        <v>2133.3609572199998</v>
+      </c>
+      <c r="AU18">
+        <v>3383.6814559999998</v>
+      </c>
+      <c r="AV18">
+        <v>1714.6517178500001</v>
+      </c>
+      <c r="AW18">
+        <v>-501.79917028</v>
+      </c>
+      <c r="AX18">
+        <v>1337.25479079</v>
+      </c>
+      <c r="AY18">
+        <v>4171.9967585499999</v>
+      </c>
+      <c r="AZ18">
+        <f t="shared" si="0"/>
+        <v>1450.0096509055802</v>
+      </c>
+      <c r="BA18">
+        <f t="shared" si="1"/>
+        <v>-6182.6028599499996</v>
+      </c>
+      <c r="BB18">
+        <f t="shared" si="2"/>
+        <v>6067.9239335299999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:54">
       <c r="A19">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>3316.6224090699998</v>
+      </c>
+      <c r="C19">
+        <v>-388.91873919099999</v>
+      </c>
+      <c r="D19">
+        <v>2001.05746823</v>
+      </c>
+      <c r="E19">
+        <v>2202.0840296199999</v>
+      </c>
+      <c r="F19">
+        <v>-309.94023832300002</v>
+      </c>
+      <c r="G19">
+        <v>1879.9287965599999</v>
+      </c>
+      <c r="H19">
+        <v>-167.269605883</v>
+      </c>
+      <c r="I19">
+        <v>2703.4874248000001</v>
+      </c>
+      <c r="J19">
+        <v>-2290.8193554300001</v>
+      </c>
+      <c r="K19">
+        <v>794.71371462800005</v>
+      </c>
+      <c r="L19">
+        <v>2236.7783937200002</v>
+      </c>
+      <c r="M19">
+        <v>-2372.6174385300001</v>
+      </c>
+      <c r="N19">
+        <v>659.53254764500002</v>
+      </c>
+      <c r="O19">
+        <v>2156.8195747999998</v>
+      </c>
+      <c r="P19">
+        <v>1401.18378437</v>
+      </c>
+      <c r="Q19">
+        <v>1660.43387272</v>
+      </c>
+      <c r="R19">
+        <v>-4584.7372215100004</v>
+      </c>
+      <c r="S19">
+        <v>1095.47133601</v>
+      </c>
+      <c r="T19">
+        <v>-436.61159805800003</v>
+      </c>
+      <c r="U19">
+        <v>711.46416515099997</v>
+      </c>
+      <c r="V19">
+        <v>1472.71052644</v>
+      </c>
+      <c r="W19">
+        <v>1427.71089394</v>
+      </c>
+      <c r="X19">
+        <v>1045.8570973599999</v>
+      </c>
+      <c r="Y19">
+        <v>1921.09191652</v>
+      </c>
+      <c r="Z19">
+        <v>1634.11278348</v>
+      </c>
+      <c r="AA19">
+        <v>-2571.0487318700002</v>
+      </c>
+      <c r="AB19">
+        <v>2715.21499984</v>
+      </c>
+      <c r="AC19">
+        <v>2480.27906575</v>
+      </c>
+      <c r="AD19">
+        <v>1038.71186339</v>
+      </c>
+      <c r="AE19">
+        <v>98.552229924299994</v>
+      </c>
+      <c r="AF19">
+        <v>1913.92576141</v>
+      </c>
+      <c r="AG19">
+        <v>1523.6244339</v>
+      </c>
+      <c r="AH19">
+        <v>-2207.0258659199999</v>
+      </c>
+      <c r="AI19">
+        <v>-477.174654858</v>
+      </c>
+      <c r="AJ19">
+        <v>1188.12036418</v>
+      </c>
+      <c r="AK19">
+        <v>460.293024629</v>
+      </c>
+      <c r="AL19">
+        <v>-67.745188612899994</v>
+      </c>
+      <c r="AM19">
+        <v>-28.069409093899999</v>
+      </c>
+      <c r="AN19">
+        <v>-236.26117928599999</v>
+      </c>
+      <c r="AO19">
+        <v>1153.03085601</v>
+      </c>
+      <c r="AP19">
+        <v>1650.62293527</v>
+      </c>
+      <c r="AQ19">
+        <v>24.4394328604</v>
+      </c>
+      <c r="AR19">
+        <v>-278.271547661</v>
+      </c>
+      <c r="AS19">
+        <v>413.87759626000002</v>
+      </c>
+      <c r="AT19">
+        <v>-427.68831187799998</v>
+      </c>
+      <c r="AU19">
+        <v>272.57215077199999</v>
+      </c>
+      <c r="AV19">
+        <v>1385.4676062799999</v>
+      </c>
+      <c r="AW19">
+        <v>2996.8203943799999</v>
+      </c>
+      <c r="AX19">
+        <v>1481.3289573899999</v>
+      </c>
+      <c r="AY19">
+        <v>-1501.9439158</v>
+      </c>
+      <c r="AZ19">
+        <f t="shared" si="0"/>
+        <v>655.43598810809783</v>
+      </c>
+      <c r="BA19">
+        <f t="shared" si="1"/>
+        <v>-4584.7372215100004</v>
+      </c>
+      <c r="BB19">
+        <f t="shared" si="2"/>
+        <v>3316.6224090699998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:54">
       <c r="A20">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>3770.96076528</v>
+      </c>
+      <c r="C20">
+        <v>1721.91584137</v>
+      </c>
+      <c r="D20">
+        <v>95.565332059400006</v>
+      </c>
+      <c r="E20">
+        <v>2946.7074380200002</v>
+      </c>
+      <c r="F20">
+        <v>-2032.1309014200001</v>
+      </c>
+      <c r="G20">
+        <v>-1293.27267936</v>
+      </c>
+      <c r="H20">
+        <v>-2627.5539136500001</v>
+      </c>
+      <c r="I20">
+        <v>1317.43024064</v>
+      </c>
+      <c r="J20">
+        <v>4552.2781133199996</v>
+      </c>
+      <c r="K20">
+        <v>-349.090995077</v>
+      </c>
+      <c r="L20">
+        <v>1370.53064795</v>
+      </c>
+      <c r="M20">
+        <v>-990.86007333700002</v>
+      </c>
+      <c r="N20">
+        <v>524.92423116500004</v>
+      </c>
+      <c r="O20">
+        <v>-149.81001568299999</v>
+      </c>
+      <c r="P20">
+        <v>3101.1593256800002</v>
+      </c>
+      <c r="Q20">
+        <v>285.76497144500001</v>
+      </c>
+      <c r="R20">
+        <v>2098.0094844700002</v>
+      </c>
+      <c r="S20">
+        <v>211.029069354</v>
+      </c>
+      <c r="T20">
+        <v>1920.83093476</v>
+      </c>
+      <c r="U20">
+        <v>1706.4529619499999</v>
+      </c>
+      <c r="V20">
+        <v>-530.652750083</v>
+      </c>
+      <c r="W20">
+        <v>828.21080181900004</v>
+      </c>
+      <c r="X20">
+        <v>1531.7070359100001</v>
+      </c>
+      <c r="Y20">
+        <v>-1526.94534368</v>
+      </c>
+      <c r="Z20">
+        <v>755.35345486200004</v>
+      </c>
+      <c r="AA20">
+        <v>2754.2049373999998</v>
+      </c>
+      <c r="AB20">
+        <v>2643.2193637800001</v>
+      </c>
+      <c r="AC20">
+        <v>-473.62875079399998</v>
+      </c>
+      <c r="AD20">
+        <v>2603.4550471299999</v>
+      </c>
+      <c r="AE20">
+        <v>5.8906415931399998</v>
+      </c>
+      <c r="AF20">
+        <v>4459.33009098</v>
+      </c>
+      <c r="AG20">
+        <v>-2342.8211424000001</v>
+      </c>
+      <c r="AH20">
+        <v>814.16073015300003</v>
+      </c>
+      <c r="AI20">
+        <v>2873.4580839300002</v>
+      </c>
+      <c r="AJ20">
+        <v>-1062.10772853</v>
+      </c>
+      <c r="AK20">
+        <v>3363.4032915100001</v>
+      </c>
+      <c r="AL20">
+        <v>2445.5511462600002</v>
+      </c>
+      <c r="AM20">
+        <v>4061.3283234999999</v>
+      </c>
+      <c r="AN20">
+        <v>-14.313439690899999</v>
+      </c>
+      <c r="AO20">
+        <v>2349.4108985799999</v>
+      </c>
+      <c r="AP20">
+        <v>176.831827143</v>
+      </c>
+      <c r="AQ20">
+        <v>-2261.0819957799999</v>
+      </c>
+      <c r="AR20">
+        <v>2748.6586470399998</v>
+      </c>
+      <c r="AS20">
+        <v>852.56977023599995</v>
+      </c>
+      <c r="AT20">
+        <v>3162.0386294599998</v>
+      </c>
+      <c r="AU20">
+        <v>-1752.57248989</v>
+      </c>
+      <c r="AV20">
+        <v>250.98388054700001</v>
+      </c>
+      <c r="AW20">
+        <v>68.369366174999996</v>
+      </c>
+      <c r="AX20">
+        <v>-2785.29421232</v>
+      </c>
+      <c r="AY20">
+        <v>2746.3337130599998</v>
+      </c>
+      <c r="AZ20">
+        <f t="shared" si="0"/>
+        <v>938.5178521367327</v>
+      </c>
+      <c r="BA20">
+        <f t="shared" si="1"/>
+        <v>-2785.29421232</v>
+      </c>
+      <c r="BB20">
+        <f t="shared" si="2"/>
+        <v>4552.2781133199996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:54">
       <c r="A21">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>622.18537576699998</v>
+      </c>
+      <c r="C21">
+        <v>-6803.3960219700002</v>
+      </c>
+      <c r="D21">
+        <v>440.966103309</v>
+      </c>
+      <c r="E21">
+        <v>231.374804058</v>
+      </c>
+      <c r="F21">
+        <v>-1476.36697177</v>
+      </c>
+      <c r="G21">
+        <v>1201.5459135900001</v>
+      </c>
+      <c r="H21">
+        <v>975.72987066899998</v>
+      </c>
+      <c r="I21">
+        <v>501.734983962</v>
+      </c>
+      <c r="J21">
+        <v>-613.83429685800002</v>
+      </c>
+      <c r="K21">
+        <v>1737.3117592900001</v>
+      </c>
+      <c r="L21">
+        <v>984.32147295599998</v>
+      </c>
+      <c r="M21">
+        <v>59.170974067400003</v>
+      </c>
+      <c r="N21">
+        <v>1633.37757143</v>
+      </c>
+      <c r="O21">
+        <v>580.46610251100003</v>
+      </c>
+      <c r="P21">
+        <v>2007.7895093699999</v>
+      </c>
+      <c r="Q21">
+        <v>1922.0377000599999</v>
+      </c>
+      <c r="R21">
+        <v>1978.12344942</v>
+      </c>
+      <c r="S21">
+        <v>471.93867494199998</v>
+      </c>
+      <c r="T21">
+        <v>1799.5914235400001</v>
+      </c>
+      <c r="U21">
+        <v>-297.681487</v>
+      </c>
+      <c r="V21">
+        <v>828.57566122799994</v>
+      </c>
+      <c r="W21">
+        <v>2975.43989547</v>
+      </c>
+      <c r="X21">
+        <v>602.77000138100004</v>
+      </c>
+      <c r="Y21">
+        <v>740.03492842100002</v>
+      </c>
+      <c r="Z21">
+        <v>1924.8693878399999</v>
+      </c>
+      <c r="AA21">
+        <v>-1902.1814311799999</v>
+      </c>
+      <c r="AB21">
+        <v>622.56647912599999</v>
+      </c>
+      <c r="AC21">
+        <v>1584.88732422</v>
+      </c>
+      <c r="AD21">
+        <v>2200.65266935</v>
+      </c>
+      <c r="AE21">
+        <v>1749.8250867500001</v>
+      </c>
+      <c r="AF21">
+        <v>798.74425441699998</v>
+      </c>
+      <c r="AG21">
+        <v>156.24778898700001</v>
+      </c>
+      <c r="AH21">
+        <v>703.35274574300001</v>
+      </c>
+      <c r="AI21">
+        <v>875.24800032899998</v>
+      </c>
+      <c r="AJ21">
+        <v>675.25941460000001</v>
+      </c>
+      <c r="AK21">
+        <v>-643.176552937</v>
+      </c>
+      <c r="AL21">
+        <v>244.021726301</v>
+      </c>
+      <c r="AM21">
+        <v>27.254043197800002</v>
+      </c>
+      <c r="AN21">
+        <v>-177.61568394299999</v>
+      </c>
+      <c r="AO21">
+        <v>268.76293239300003</v>
+      </c>
+      <c r="AP21">
+        <v>3027.8379280099998</v>
+      </c>
+      <c r="AQ21">
+        <v>2733.6939881600001</v>
+      </c>
+      <c r="AR21">
+        <v>-688.87940531200002</v>
+      </c>
+      <c r="AS21">
+        <v>-2516.9976338699998</v>
+      </c>
+      <c r="AT21">
+        <v>2451.12019676</v>
+      </c>
+      <c r="AU21">
+        <v>956.08847914600005</v>
+      </c>
+      <c r="AV21">
+        <v>-373.36888719400002</v>
+      </c>
+      <c r="AW21">
+        <v>1624.58615781</v>
+      </c>
+      <c r="AX21">
+        <v>940.12174162300005</v>
+      </c>
+      <c r="AY21">
+        <v>-2252.21061732</v>
+      </c>
+      <c r="AZ21">
+        <f t="shared" si="0"/>
+        <v>562.27835061700421</v>
+      </c>
+      <c r="BA21">
+        <f t="shared" si="1"/>
+        <v>-6803.3960219700002</v>
+      </c>
+      <c r="BB21">
+        <f t="shared" si="2"/>
+        <v>3027.8379280099998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:54">
       <c r="A22">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>-1425.4982926</v>
+      </c>
+      <c r="C22">
+        <v>2352.7197949900001</v>
+      </c>
+      <c r="D22">
+        <v>1816.0949051499999</v>
+      </c>
+      <c r="E22">
+        <v>1086.4756640400001</v>
+      </c>
+      <c r="F22">
+        <v>1653.4284087399999</v>
+      </c>
+      <c r="G22">
+        <v>2477.33406844</v>
+      </c>
+      <c r="H22">
+        <v>105.007612947</v>
+      </c>
+      <c r="I22">
+        <v>-600.94917281799997</v>
+      </c>
+      <c r="J22">
+        <v>1355.5800345800001</v>
+      </c>
+      <c r="K22">
+        <v>5517.0850720600001</v>
+      </c>
+      <c r="L22">
+        <v>-2806.6879527999999</v>
+      </c>
+      <c r="M22">
+        <v>-5391.1969596600002</v>
+      </c>
+      <c r="N22">
+        <v>1088.91594459</v>
+      </c>
+      <c r="O22">
+        <v>-2931.1276869200001</v>
+      </c>
+      <c r="P22">
+        <v>-26.4047160139</v>
+      </c>
+      <c r="Q22">
+        <v>1203.5260849599999</v>
+      </c>
+      <c r="R22">
+        <v>853.14391440600002</v>
+      </c>
+      <c r="S22">
+        <v>-3929.64087397</v>
+      </c>
+      <c r="T22">
+        <v>2485.0855648699999</v>
+      </c>
+      <c r="U22">
+        <v>2884.1938670700001</v>
+      </c>
+      <c r="V22">
+        <v>2517.4387503100002</v>
+      </c>
+      <c r="W22">
+        <v>-36.9691753838</v>
+      </c>
+      <c r="X22">
+        <v>2046.0502883700001</v>
+      </c>
+      <c r="Y22">
+        <v>6819.1457754200001</v>
+      </c>
+      <c r="Z22">
+        <v>3696.51292797</v>
+      </c>
+      <c r="AA22">
+        <v>-6781.1558560200001</v>
+      </c>
+      <c r="AB22">
+        <v>-1971.0581781599999</v>
+      </c>
+      <c r="AC22">
+        <v>-1626.12463748</v>
+      </c>
+      <c r="AD22">
+        <v>755.96277083999996</v>
+      </c>
+      <c r="AE22">
+        <v>53.977604077400002</v>
+      </c>
+      <c r="AF22">
+        <v>3894.1198987399998</v>
+      </c>
+      <c r="AG22">
+        <v>4208.7280755800002</v>
+      </c>
+      <c r="AH22">
+        <v>1553.8131885400001</v>
+      </c>
+      <c r="AI22">
+        <v>1210.76749382</v>
+      </c>
+      <c r="AJ22">
+        <v>4596.6691293100002</v>
+      </c>
+      <c r="AK22">
+        <v>5512.0402553499998</v>
+      </c>
+      <c r="AL22">
+        <v>-1013.80761913</v>
+      </c>
+      <c r="AM22">
+        <v>2354.47492526</v>
+      </c>
+      <c r="AN22">
+        <v>2700.2661133299998</v>
+      </c>
+      <c r="AO22">
+        <v>997.80225117299995</v>
+      </c>
+      <c r="AP22">
+        <v>-1006.9161529</v>
+      </c>
+      <c r="AQ22">
+        <v>1303.8715835099999</v>
+      </c>
+      <c r="AR22">
+        <v>4553.1512268699998</v>
+      </c>
+      <c r="AS22">
+        <v>1746.0199092600001</v>
+      </c>
+      <c r="AT22">
+        <v>-46.131138401100003</v>
+      </c>
+      <c r="AU22">
+        <v>-68.341903502600005</v>
+      </c>
+      <c r="AV22">
+        <v>611.94809633700004</v>
+      </c>
+      <c r="AW22">
+        <v>-1745.50058315</v>
+      </c>
+      <c r="AX22">
+        <v>1276.0056674299999</v>
+      </c>
+      <c r="AY22">
+        <v>-193.24698029800001</v>
+      </c>
+      <c r="AZ22">
+        <f t="shared" si="0"/>
+        <v>913.73197978266035</v>
+      </c>
+      <c r="BA22">
+        <f t="shared" si="1"/>
+        <v>-6781.1558560200001</v>
+      </c>
+      <c r="BB22">
+        <f t="shared" si="2"/>
+        <v>6819.1457754200001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:54">
       <c r="A23">
         <v>20</v>
       </c>
+      <c r="B23">
+        <v>1425.73103657</v>
+      </c>
+      <c r="C23">
+        <v>1940.09784092</v>
+      </c>
+      <c r="D23">
+        <v>1585.45513265</v>
+      </c>
+      <c r="E23">
+        <v>670.03304262899997</v>
+      </c>
+      <c r="F23">
+        <v>3057.91787393</v>
+      </c>
+      <c r="G23">
+        <v>-5439.9496793199996</v>
+      </c>
+      <c r="H23">
+        <v>616.05889092100006</v>
+      </c>
+      <c r="I23">
+        <v>158.94152525000001</v>
+      </c>
+      <c r="J23">
+        <v>1219.5844377200001</v>
+      </c>
+      <c r="K23">
+        <v>-31.021833877199999</v>
+      </c>
+      <c r="L23">
+        <v>1230.4593511999999</v>
+      </c>
+      <c r="M23">
+        <v>1370.1312211699999</v>
+      </c>
+      <c r="N23">
+        <v>2857.2773647899999</v>
+      </c>
+      <c r="O23">
+        <v>1100</v>
+      </c>
+      <c r="P23">
+        <v>3087.0605034499999</v>
+      </c>
+      <c r="Q23">
+        <v>4677.1233369299998</v>
+      </c>
+      <c r="R23">
+        <v>3778.7815834500002</v>
+      </c>
+      <c r="S23">
+        <v>1040.34196299</v>
+      </c>
+      <c r="T23">
+        <v>567.44195587199999</v>
+      </c>
+      <c r="U23">
+        <v>1907.4860847899999</v>
+      </c>
+      <c r="V23">
+        <v>-636.99262848199999</v>
+      </c>
+      <c r="W23">
+        <v>195.645115401</v>
+      </c>
+      <c r="X23">
+        <v>1219.8195252999999</v>
+      </c>
+      <c r="Y23">
+        <v>1268.32999625</v>
+      </c>
+      <c r="Z23">
+        <v>826.17558246399994</v>
+      </c>
+      <c r="AA23">
+        <v>-1404.9816510799999</v>
+      </c>
+      <c r="AB23">
+        <v>1350.6550048399999</v>
+      </c>
+      <c r="AC23">
+        <v>759.48286185699999</v>
+      </c>
+      <c r="AD23">
+        <v>2116.33813551</v>
+      </c>
+      <c r="AE23">
+        <v>826.29285602000004</v>
+      </c>
+      <c r="AF23">
+        <v>593.37490431000003</v>
+      </c>
+      <c r="AG23">
+        <v>-373.10258431699998</v>
+      </c>
+      <c r="AH23">
+        <v>-1960.2488982100001</v>
+      </c>
+      <c r="AI23">
+        <v>1056.1361759900001</v>
+      </c>
+      <c r="AJ23">
+        <v>1381.6998784299999</v>
+      </c>
+      <c r="AK23">
+        <v>956.37495314399996</v>
+      </c>
+      <c r="AL23">
+        <v>-1480.3314296399999</v>
+      </c>
+      <c r="AM23">
+        <v>2545.7163412199998</v>
+      </c>
+      <c r="AN23">
+        <v>2692.8498458700001</v>
+      </c>
+      <c r="AO23">
+        <v>1593.6492893100001</v>
+      </c>
+      <c r="AP23">
+        <v>1318.1540433099999</v>
+      </c>
+      <c r="AQ23">
+        <v>3104.60154044</v>
+      </c>
+      <c r="AR23">
+        <v>1980.0170240299999</v>
+      </c>
+      <c r="AS23">
+        <v>758.35747924700001</v>
+      </c>
+      <c r="AT23">
+        <v>-1819.93467491</v>
+      </c>
+      <c r="AU23">
+        <v>3826.0763124300001</v>
+      </c>
+      <c r="AV23">
+        <v>-42.991301934299997</v>
+      </c>
+      <c r="AW23">
+        <v>-587.99870589600005</v>
+      </c>
+      <c r="AX23">
+        <v>2019.1836272</v>
+      </c>
+      <c r="AY23">
+        <v>-2510.6306640799999</v>
+      </c>
+      <c r="AZ23">
+        <f t="shared" si="0"/>
+        <v>967.81339172117009</v>
+      </c>
+      <c r="BA23">
+        <f t="shared" si="1"/>
+        <v>-5439.9496793199996</v>
+      </c>
+      <c r="BB23">
+        <f t="shared" si="2"/>
+        <v>4677.1233369299998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>